<commit_message>
Ajustes IM e Nova Planilha IP-CUC3.XLSX para José/Willas
</commit_message>
<xml_diff>
--- a/outputs/autoaprop.xlsx/autoapropxlsx/IMC1.XLSX
+++ b/outputs/autoaprop.xlsx/autoapropxlsx/IMC1.XLSX
@@ -166,7 +166,7 @@
     <t> </t>
   </si>
   <si>
-    <t>SETOR  IMC</t>
+    <t>SETOR IMC</t>
   </si>
   <si>
     <t>IMC1</t>
@@ -6093,7 +6093,7 @@
     <row r="1" spans="1:40" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="110" t="str">
         <f>'Segunda a Sexta'!A1:E9</f>
-        <v>SETOR  IMC</v>
+        <v>SETOR IMC</v>
       </c>
       <c r="B1" s="111"/>
       <c r="C1" s="111"/>

</xml_diff>